<commit_message>
Added some CES information to the US and UK Excel workbooks. Added a footnote about Stern and Kander's equation being wrong in the text of their 2012 paper.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/UnitedKingdomDataWorkbook.xlsx
+++ b/data/Excel Workbooks/UnitedKingdomDataWorkbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="340" windowWidth="24000" windowHeight="17100" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="340" windowWidth="26800" windowHeight="17100" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="UK Workbook" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,20 @@
     <sheet name="Capital Stock Comparison" sheetId="4" r:id="rId8"/>
     <sheet name="GDP Comparison Graph" sheetId="7" r:id="rId9"/>
     <sheet name="GDP Comparison" sheetId="6" r:id="rId10"/>
+    <sheet name="CES Models" sheetId="14" r:id="rId11"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId12"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="alpha">'CES Models'!$K$9</definedName>
+    <definedName name="beta">'CES Models'!$K$3</definedName>
+    <definedName name="gamma_E">'CES Models'!$K$2</definedName>
+    <definedName name="invPhi">'CES Models'!$K$7</definedName>
+    <definedName name="lambda_E">'CES Models'!$K$5</definedName>
+    <definedName name="lambda_L">'CES Models'!$K$4</definedName>
+    <definedName name="phi">'CES Models'!$K$6</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -28,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="161">
   <si>
     <t>GDP [Millions of 1990$]</t>
   </si>
@@ -1070,6 +1083,60 @@
   <si>
     <t>UK</t>
   </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>A_L</t>
+  </si>
+  <si>
+    <t>A_E</t>
+  </si>
+  <si>
+    <t>CD term</t>
+  </si>
+  <si>
+    <t>Using Q</t>
+  </si>
+  <si>
+    <t>Using X</t>
+  </si>
+  <si>
+    <t>Using U</t>
+  </si>
+  <si>
+    <t>gamma_E</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>lambda_L</t>
+  </si>
+  <si>
+    <t>lambda_E</t>
+  </si>
+  <si>
+    <t>(sigma-1)/sigma</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>sigma/(sigma-1)</t>
+  </si>
+  <si>
+    <t>invPhi</t>
+  </si>
+  <si>
+    <t>1/sigma</t>
+  </si>
+  <si>
+    <t>invSigma</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
 </sst>
 </file>
 
@@ -1086,7 +1153,7 @@
     <numFmt numFmtId="170" formatCode="0.0%"/>
     <numFmt numFmtId="171" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1444,8 +1511,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="47">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1693,6 +1767,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -5965,7 +6045,7 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6292,12 +6372,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6310,7 +6384,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6322,6 +6402,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3841">
     <cellStyle name="•\Ž¦Ï‚Ý‚ÌƒnƒCƒp[ƒŠƒ“ƒN" xfId="45"/>
@@ -11608,11 +11690,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2144291000"/>
-        <c:axId val="-2144298888"/>
+        <c:axId val="2132501320"/>
+        <c:axId val="2132646696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2144291000"/>
+        <c:axId val="2132501320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015.0"/>
@@ -11642,12 +11724,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144298888"/>
+        <c:crossAx val="2132646696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2144298888"/>
+        <c:axId val="2132646696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -11681,7 +11763,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144291000"/>
+        <c:crossAx val="2132501320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -12634,11 +12716,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2143159880"/>
-        <c:axId val="-2143168168"/>
+        <c:axId val="2131861928"/>
+        <c:axId val="2132639688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2143159880"/>
+        <c:axId val="2131861928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2011.0"/>
@@ -12668,13 +12750,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143168168"/>
+        <c:crossAx val="2132639688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2143168168"/>
+        <c:axId val="2132639688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -12723,7 +12805,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143159880"/>
+        <c:crossAx val="2131861928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14477,11 +14559,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2141728456"/>
-        <c:axId val="-2141720600"/>
+        <c:axId val="2134090680"/>
+        <c:axId val="2134098600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2141728456"/>
+        <c:axId val="2134090680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2011.0"/>
@@ -14511,13 +14593,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141720600"/>
+        <c:crossAx val="2134098600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141720600"/>
+        <c:axId val="2134098600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14545,7 +14627,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141728456"/>
+        <c:crossAx val="2134090680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14558,6 +14640,974 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Historical GDP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CES Models'!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1980.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1981.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1982.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1983.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1984.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1985.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1986.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1987.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1988.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1989.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1990.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1991.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1992.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1993.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1995.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1996.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1997.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1998.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1999.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2001.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2002.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2003.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CES Models'!$C$2:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.986773691064354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.007419866725305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.043930240393394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.071811964888728</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.110396129152832</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.154949621205302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.207642248403936</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.268409713810039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.297350194562536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.307461959787837</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.289253924042169</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.291144254039777</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.31983954913272</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.376332554054436</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.418340744627133</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.459263602874673</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.509218895069968</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.567158152466045</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.624448439427569</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.696860509077442</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.750322984955374</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.796837962284273</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.8601695896055</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.915143472189002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.955089016968391</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.006061058087569</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.075594339468976</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.052702914708825</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.962931528904046</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.003999269586776</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.017119274250448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>With q</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CES Models'!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1980.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1981.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1982.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1983.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1984.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1985.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1986.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1987.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1988.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1989.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1990.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1991.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1992.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1993.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1995.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1996.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1997.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1998.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1999.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2001.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2002.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2003.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CES Models'!$P$2:$P$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.983961678028219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.988928762683452</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.005303902353804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.035722758999154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.081555786435808</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.117122259976324</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.160917816182592</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.212243326080428</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.271338928615585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.304270817064145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.325942452330193</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.328146937077421</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.36267154159789</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.406738184020825</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.445029721599703</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.541460085498715</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.560057316878255</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.609849941534577</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.659568015985913</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.698649302302861</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.771257999481756</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.805046862141568</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.863459184096126</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.92082875983329</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.97946181185331</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.020683657284417</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.02823161749014</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.069728432343267</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.040240239089627</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.114917354054744</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.100346201569756</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>With x</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CES Models'!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1980.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1981.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1982.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1983.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1984.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1985.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1986.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1987.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1988.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1989.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1990.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1991.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1992.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1993.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1995.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1996.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1997.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1998.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1999.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2001.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2002.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2003.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CES Models'!$Q$2:$Q$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.985210927213528</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.993135214169333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.014293716524796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.039767537046623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.096269446619188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.139922667202862</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.185979031405023</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.233757484787347</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.296415712840116</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.333780668247458</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.373177832488544</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.377077407299598</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.420670646513761</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.468595900469691</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.507939795821793</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.62610000227381</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.637128151497511</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.690611160720098</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.743443621716883</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.784681491689048</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.867575183192886</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.902722308827353</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.968966260648677</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.03144826709386</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.09413875326611</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.136461767810835</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.131946381990418</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.174042047800603</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.136328558313194</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.224715098516776</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.197305546390846</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>With u</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CES Models'!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1980.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1981.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1982.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1983.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1984.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1985.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1986.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1987.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1988.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1989.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1990.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1991.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1992.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1993.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1995.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1996.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1997.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1998.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1999.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2001.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2002.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2003.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CES Models'!$R$2:$R$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98939815530155</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.986301306162648</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.021229293200982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.076343037552158</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.120054660289398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.166456064276459</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.25326751722906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.311943778821283</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.375368165123735</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.436811067725533</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.451098635624046</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.525628253306313</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.579822382920155</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.771532937025222</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.822594014290764</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.947585464817141</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.961329662129059</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.055083485824728</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.082320875888715</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.232921889777649</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2130794424"/>
+        <c:axId val="2131102072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2130794424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2131102072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2131102072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2130794424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -15267,6 +16317,585 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="United States Workbook"/>
+      <sheetName val="USData"/>
+      <sheetName val="US Indices Comparison"/>
+      <sheetName val="Labour calculations"/>
+      <sheetName val="Exergy calcs"/>
+      <sheetName val="Useful work calcs"/>
+      <sheetName val="Capital Stock Comparison Graph"/>
+      <sheetName val="Capital Stock Comparison"/>
+      <sheetName val="GDP Comparison Graph"/>
+      <sheetName val="GDP Comparison"/>
+      <sheetName val="CES models"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10">
+        <row r="2">
+          <cell r="A2">
+            <v>1980</v>
+          </cell>
+          <cell r="C2">
+            <v>1</v>
+          </cell>
+          <cell r="P2">
+            <v>1</v>
+          </cell>
+          <cell r="Q2">
+            <v>1</v>
+          </cell>
+          <cell r="R2">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>1981</v>
+          </cell>
+          <cell r="C3">
+            <v>1.0253857789928822</v>
+          </cell>
+          <cell r="P3">
+            <v>1.0204736215500438</v>
+          </cell>
+          <cell r="Q3">
+            <v>1.0203680908554074</v>
+          </cell>
+          <cell r="R3">
+            <v>1.0202306018014293</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>1982</v>
+          </cell>
+          <cell r="C4">
+            <v>1.0054765404376946</v>
+          </cell>
+          <cell r="P4">
+            <v>1.0258396382572177</v>
+          </cell>
+          <cell r="Q4">
+            <v>1.0256899820668377</v>
+          </cell>
+          <cell r="R4">
+            <v>1.0255237079030171</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>1983</v>
+          </cell>
+          <cell r="C5">
+            <v>1.0509001152730342</v>
+          </cell>
+          <cell r="P5">
+            <v>1.0572887745364343</v>
+          </cell>
+          <cell r="Q5">
+            <v>1.0571226163790735</v>
+          </cell>
+          <cell r="R5">
+            <v>1.0569474056228705</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>1984</v>
+          </cell>
+          <cell r="C6">
+            <v>1.1264232363011497</v>
+          </cell>
+          <cell r="P6">
+            <v>1.1186468206858819</v>
+          </cell>
+          <cell r="Q6">
+            <v>1.1184827499997807</v>
+          </cell>
+          <cell r="R6">
+            <v>1.1183069963859926</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>1985</v>
+          </cell>
+          <cell r="C7">
+            <v>1.1730252529364626</v>
+          </cell>
+          <cell r="P7">
+            <v>1.1615797656379097</v>
+          </cell>
+          <cell r="Q7">
+            <v>1.1613950569165381</v>
+          </cell>
+          <cell r="R7">
+            <v>1.1612104564787413</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>1986</v>
+          </cell>
+          <cell r="C8">
+            <v>1.2136664966853645</v>
+          </cell>
+          <cell r="P8">
+            <v>1.1958062473635533</v>
+          </cell>
+          <cell r="Q8">
+            <v>1.195613438838903</v>
+          </cell>
+          <cell r="R8">
+            <v>1.1954167121773991</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1987</v>
+          </cell>
+          <cell r="C9">
+            <v>1.2524993679266709</v>
+          </cell>
+          <cell r="P9">
+            <v>1.2436555272562895</v>
+          </cell>
+          <cell r="Q9">
+            <v>1.2434648204059637</v>
+          </cell>
+          <cell r="R9">
+            <v>1.2432683685025845</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>1988</v>
+          </cell>
+          <cell r="C10">
+            <v>1.3039822762353284</v>
+          </cell>
+          <cell r="P10">
+            <v>1.2957939540283201</v>
+          </cell>
+          <cell r="Q10">
+            <v>1.2956355493647942</v>
+          </cell>
+          <cell r="R10">
+            <v>1.2955271333901193</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>1989</v>
+          </cell>
+          <cell r="C11">
+            <v>1.3505671518990054</v>
+          </cell>
+          <cell r="P11">
+            <v>1.3479025060598049</v>
+          </cell>
+          <cell r="Q11">
+            <v>1.3477770577594308</v>
+          </cell>
+          <cell r="R11">
+            <v>1.3480618663282531</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1990</v>
+          </cell>
+          <cell r="C12">
+            <v>1.3759100784627976</v>
+          </cell>
+          <cell r="P12">
+            <v>1.3747933249920963</v>
+          </cell>
+          <cell r="Q12">
+            <v>1.3746976473463661</v>
+          </cell>
+          <cell r="R12">
+            <v>1.3755624562599085</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>1991</v>
+          </cell>
+          <cell r="C13">
+            <v>1.37270471676687</v>
+          </cell>
+          <cell r="P13">
+            <v>1.3832137716976249</v>
+          </cell>
+          <cell r="Q13">
+            <v>1.3832341216856923</v>
+          </cell>
+          <cell r="R13">
+            <v>1.3843083616339238</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>1992</v>
+          </cell>
+          <cell r="C14">
+            <v>1.41927673670182</v>
+          </cell>
+          <cell r="P14">
+            <v>1.4082301382342552</v>
+          </cell>
+          <cell r="Q14">
+            <v>1.4085315460038599</v>
+          </cell>
+          <cell r="R14">
+            <v>1.4160317854407301</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>1993</v>
+          </cell>
+          <cell r="C15">
+            <v>1.4597551412201801</v>
+          </cell>
+          <cell r="P15">
+            <v>1.4585823658919383</v>
+          </cell>
+          <cell r="Q15">
+            <v>1.45903325052458</v>
+          </cell>
+          <cell r="R15">
+            <v>1.465813727971905</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>1994</v>
+          </cell>
+          <cell r="C16">
+            <v>1.519225742311203</v>
+          </cell>
+          <cell r="P16">
+            <v>1.5209334832863295</v>
+          </cell>
+          <cell r="Q16">
+            <v>1.5213719754703734</v>
+          </cell>
+          <cell r="R16">
+            <v>1.5323700014114352</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>1995</v>
+          </cell>
+          <cell r="C17">
+            <v>1.5574243976019781</v>
+          </cell>
+          <cell r="P17">
+            <v>1.5799261041795343</v>
+          </cell>
+          <cell r="Q17">
+            <v>1.5805307983871659</v>
+          </cell>
+          <cell r="R17">
+            <v>1.6072462701191914</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>1996</v>
+          </cell>
+          <cell r="C18">
+            <v>1.6156822749497555</v>
+          </cell>
+          <cell r="P18">
+            <v>1.6307284911297213</v>
+          </cell>
+          <cell r="Q18">
+            <v>1.6326459067009078</v>
+          </cell>
+          <cell r="R18">
+            <v>1.6811550747054322</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>1997</v>
+          </cell>
+          <cell r="C19">
+            <v>1.6876872115495867</v>
+          </cell>
+          <cell r="P19">
+            <v>1.7029795236792338</v>
+          </cell>
+          <cell r="Q19">
+            <v>1.704042984943352</v>
+          </cell>
+          <cell r="R19">
+            <v>1.7460845792467194</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>1998</v>
+          </cell>
+          <cell r="C20">
+            <v>1.7611919831675658</v>
+          </cell>
+          <cell r="P20">
+            <v>1.7724064362271621</v>
+          </cell>
+          <cell r="Q20">
+            <v>1.7729783328829083</v>
+          </cell>
+          <cell r="R20">
+            <v>1.8086661664064663</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>1999</v>
+          </cell>
+          <cell r="C21">
+            <v>1.8461897762674677</v>
+          </cell>
+          <cell r="P21">
+            <v>1.8447987851443208</v>
+          </cell>
+          <cell r="Q21">
+            <v>1.8452989159947781</v>
+          </cell>
+          <cell r="R21">
+            <v>1.8964476649164279</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>2000</v>
+          </cell>
+          <cell r="C22">
+            <v>1.9226042278206541</v>
+          </cell>
+          <cell r="P22">
+            <v>1.9128560525642373</v>
+          </cell>
+          <cell r="Q22">
+            <v>1.9136189768293614</v>
+          </cell>
+          <cell r="R22">
+            <v>1.9405119932307708</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>2001</v>
+          </cell>
+          <cell r="C23">
+            <v>1.9433533739860045</v>
+          </cell>
+          <cell r="P23">
+            <v>1.9410869139354936</v>
+          </cell>
+          <cell r="Q23">
+            <v>1.941311580975815</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>2002</v>
+          </cell>
+          <cell r="C24">
+            <v>1.9785994969124825</v>
+          </cell>
+          <cell r="P24">
+            <v>1.9649820658088395</v>
+          </cell>
+          <cell r="Q24">
+            <v>1.966331666465913</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>2003</v>
+          </cell>
+          <cell r="C25">
+            <v>2.0288782519637127</v>
+          </cell>
+          <cell r="P25">
+            <v>1.9995546343483528</v>
+          </cell>
+          <cell r="Q25">
+            <v>2.0014276737644066</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>2004</v>
+          </cell>
+          <cell r="C26">
+            <v>2.0992419405293989</v>
+          </cell>
+          <cell r="P26">
+            <v>2.061386958998451</v>
+          </cell>
+          <cell r="Q26">
+            <v>2.0641215142971117</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>2005</v>
+          </cell>
+          <cell r="C27">
+            <v>2.1636962791235823</v>
+          </cell>
+          <cell r="P27">
+            <v>2.13043897797295</v>
+          </cell>
+          <cell r="Q27">
+            <v>2.1321915962558844</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>2006</v>
+          </cell>
+          <cell r="C28">
+            <v>2.2212085242051947</v>
+          </cell>
+          <cell r="P28">
+            <v>2.2049028499886405</v>
+          </cell>
+          <cell r="Q28">
+            <v>2.2055366663613434</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>2007</v>
+          </cell>
+          <cell r="C29">
+            <v>2.2637009928907821</v>
+          </cell>
+          <cell r="P29">
+            <v>2.2616989357881314</v>
+          </cell>
+          <cell r="Q29">
+            <v>2.263045948176289</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>2008</v>
+          </cell>
+          <cell r="C30">
+            <v>2.2560818309985899</v>
+          </cell>
+          <cell r="P30">
+            <v>2.2818543088894514</v>
+          </cell>
+          <cell r="Q30">
+            <v>2.2825619266122987</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>2009</v>
+          </cell>
+          <cell r="C31">
+            <v>2.1774390531327268</v>
+          </cell>
+          <cell r="P31">
+            <v>2.2160813457043989</v>
+          </cell>
+          <cell r="Q31">
+            <v>2.2169806645566514</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>2010</v>
+          </cell>
+          <cell r="C32">
+            <v>2.2434060824737849</v>
+          </cell>
+          <cell r="P32">
+            <v>2.2494521352935246</v>
+          </cell>
+          <cell r="Q32">
+            <v>2.2553014933279099</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>2011</v>
+          </cell>
+          <cell r="C33">
+            <v>2.2823332290590894</v>
+          </cell>
+          <cell r="P33">
+            <v>2.3267584930386085</v>
+          </cell>
+          <cell r="Q33">
+            <v>2.3289156298921472</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -17410,18 +19039,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L8:L9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -17437,7 +19066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -19642,13 +21271,13 @@
       </c>
     </row>
     <row r="28" spans="1:39" ht="15" customHeight="1">
-      <c r="A28" s="140" t="s">
+      <c r="A28" s="138" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="142" t="s">
+      <c r="C28" s="140" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="136" t="s">
@@ -19676,11 +21305,11 @@
         <v>72</v>
       </c>
       <c r="L28" s="136"/>
-      <c r="M28" s="138"/>
-      <c r="N28" s="140" t="s">
+      <c r="M28" s="142"/>
+      <c r="N28" s="138" t="s">
         <v>58</v>
       </c>
-      <c r="O28" s="142" t="s">
+      <c r="O28" s="140" t="s">
         <v>59</v>
       </c>
       <c r="P28" s="136" t="s">
@@ -19690,11 +21319,11 @@
         <v>83</v>
       </c>
       <c r="R28" s="136"/>
-      <c r="S28" s="138"/>
-      <c r="T28" s="140" t="s">
+      <c r="S28" s="142"/>
+      <c r="T28" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="U28" s="142" t="s">
+      <c r="U28" s="140" t="s">
         <v>29</v>
       </c>
       <c r="V28" s="136" t="s">
@@ -19716,13 +21345,13 @@
         <v>82</v>
       </c>
       <c r="AB28" s="136"/>
-      <c r="AC28" s="138" t="s">
+      <c r="AC28" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="AD28" s="140" t="s">
+      <c r="AD28" s="138" t="s">
         <v>85</v>
       </c>
-      <c r="AE28" s="142" t="s">
+      <c r="AE28" s="140" t="s">
         <v>86</v>
       </c>
       <c r="AF28" s="136" t="s">
@@ -19744,14 +21373,14 @@
         <v>92</v>
       </c>
       <c r="AL28" s="136"/>
-      <c r="AM28" s="138" t="s">
+      <c r="AM28" s="142" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:39">
-      <c r="A29" s="141"/>
+      <c r="A29" s="139"/>
       <c r="B29" s="137"/>
-      <c r="C29" s="143"/>
+      <c r="C29" s="141"/>
       <c r="D29" s="137"/>
       <c r="E29" s="137"/>
       <c r="F29" s="137"/>
@@ -19761,15 +21390,15 @@
       <c r="J29" s="137"/>
       <c r="K29" s="137"/>
       <c r="L29" s="137"/>
-      <c r="M29" s="144"/>
-      <c r="N29" s="141"/>
-      <c r="O29" s="143"/>
+      <c r="M29" s="143"/>
+      <c r="N29" s="139"/>
+      <c r="O29" s="141"/>
       <c r="P29" s="137"/>
       <c r="Q29" s="137"/>
       <c r="R29" s="137"/>
-      <c r="S29" s="144"/>
-      <c r="T29" s="141"/>
-      <c r="U29" s="143"/>
+      <c r="S29" s="143"/>
+      <c r="T29" s="139"/>
+      <c r="U29" s="141"/>
       <c r="V29" s="137"/>
       <c r="W29" s="137"/>
       <c r="X29" s="137"/>
@@ -19777,9 +21406,9 @@
       <c r="Z29" s="137"/>
       <c r="AA29" s="137"/>
       <c r="AB29" s="137"/>
-      <c r="AC29" s="139"/>
-      <c r="AD29" s="141"/>
-      <c r="AE29" s="143"/>
+      <c r="AC29" s="144"/>
+      <c r="AD29" s="139"/>
+      <c r="AE29" s="141"/>
       <c r="AF29" s="137"/>
       <c r="AG29" s="137"/>
       <c r="AH29" s="137"/>
@@ -19787,7 +21416,7 @@
       <c r="AJ29" s="137"/>
       <c r="AK29" s="137"/>
       <c r="AL29" s="137"/>
-      <c r="AM29" s="139"/>
+      <c r="AM29" s="144"/>
     </row>
     <row r="30" spans="1:39">
       <c r="A30" s="56">
@@ -23736,14 +25365,25 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="AI28:AI29"/>
+    <mergeCell ref="AJ28:AJ29"/>
+    <mergeCell ref="AK28:AK29"/>
+    <mergeCell ref="AL28:AL29"/>
+    <mergeCell ref="AM28:AM29"/>
+    <mergeCell ref="AD28:AD29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="AH28:AH29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AB28:AB29"/>
+    <mergeCell ref="AC28:AC29"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="V28:V29"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="Z28:Z29"/>
     <mergeCell ref="T28:T29"/>
     <mergeCell ref="I28:I29"/>
     <mergeCell ref="J28:J29"/>
@@ -23756,25 +25396,14 @@
     <mergeCell ref="Q28:Q29"/>
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AB28:AB29"/>
-    <mergeCell ref="AC28:AC29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="V28:V29"/>
-    <mergeCell ref="W28:W29"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="AE28:AE29"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="AH28:AH29"/>
-    <mergeCell ref="AI28:AI29"/>
-    <mergeCell ref="AJ28:AJ29"/>
-    <mergeCell ref="AK28:AK29"/>
-    <mergeCell ref="AL28:AL29"/>
-    <mergeCell ref="AM28:AM29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -35462,17 +37091,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="E5:G6"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -35481,4 +37110,2298 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="148" t="str">
+        <f>UKData!A1</f>
+        <v>Year</v>
+      </c>
+      <c r="B1" s="148" t="str">
+        <f>UKData!B1</f>
+        <v>iYear</v>
+      </c>
+      <c r="C1" s="148" t="str">
+        <f>UKData!C1</f>
+        <v>iGDP</v>
+      </c>
+      <c r="D1" s="148" t="str">
+        <f>UKData!D1</f>
+        <v>iLabor</v>
+      </c>
+      <c r="E1" s="148" t="str">
+        <f>UKData!E1</f>
+        <v>iCapStk</v>
+      </c>
+      <c r="F1" s="148" t="str">
+        <f>UKData!F1</f>
+        <v>iQ</v>
+      </c>
+      <c r="G1" s="148" t="str">
+        <f>UKData!G1</f>
+        <v>iX</v>
+      </c>
+      <c r="H1" s="148" t="str">
+        <f>UKData!H1</f>
+        <v>iU</v>
+      </c>
+      <c r="I1" s="148"/>
+      <c r="J1" s="148" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="149">
+        <v>-0.2</v>
+      </c>
+      <c r="L1" s="148"/>
+      <c r="M1" s="148" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" s="148" t="s">
+        <v>145</v>
+      </c>
+      <c r="O1" s="148" t="s">
+        <v>146</v>
+      </c>
+      <c r="P1" s="148" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q1" s="148" t="s">
+        <v>148</v>
+      </c>
+      <c r="R1" s="148" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="148">
+        <f>UKData!A2</f>
+        <v>1980</v>
+      </c>
+      <c r="B2" s="148">
+        <f>UKData!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="148">
+        <f>UKData!C2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="148">
+        <f>UKData!D2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="148">
+        <f>UKData!E2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="148">
+        <f>UKData!F2</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="148">
+        <f>UKData!G2</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="148">
+        <f>UKData!H2</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="149">
+        <v>0.24</v>
+      </c>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148">
+        <f>EXP(lambda_L*B2)</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="148">
+        <f>EXP(lambda_E*B2)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="148">
+        <f>E2^alpha * (M2*D2)^beta</f>
+        <v>1</v>
+      </c>
+      <c r="P2" s="148">
+        <f>((1-gamma_E)^1 * O2^phi + gamma_E^1 * ($N2*F2)^phi)^invPhi</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="148">
+        <f>((1-gamma_E)^1 * P2^phi + gamma_E^1 * ($N2*G2)^phi)^invPhi</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="148">
+        <f>((1-gamma_E)^1 * Q2^phi + gamma_E^1 * ($N2*H2)^phi)^invPhi</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="148">
+        <f>UKData!A3</f>
+        <v>1981</v>
+      </c>
+      <c r="B3" s="148">
+        <f>UKData!B3</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="148">
+        <f>UKData!C3</f>
+        <v>0.98677369106435442</v>
+      </c>
+      <c r="D3" s="148">
+        <f>UKData!D3</f>
+        <v>0.95413909207012659</v>
+      </c>
+      <c r="E3" s="148">
+        <f>UKData!E3</f>
+        <v>1.0183519235909098</v>
+      </c>
+      <c r="F3" s="148">
+        <f>UKData!F3</f>
+        <v>0.96065348946764595</v>
+      </c>
+      <c r="G3" s="148">
+        <f>UKData!G3</f>
+        <v>0.95988269283847505</v>
+      </c>
+      <c r="H3" s="148">
+        <f>UKData!H3</f>
+        <v>0.97248665671774581</v>
+      </c>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148" t="s">
+        <v>151</v>
+      </c>
+      <c r="K3" s="149">
+        <v>0.71</v>
+      </c>
+      <c r="L3" s="148"/>
+      <c r="M3" s="148">
+        <f>EXP(lambda_L*B3)</f>
+        <v>1.0140984589384923</v>
+      </c>
+      <c r="N3" s="148">
+        <f>EXP(lambda_E*B3)</f>
+        <v>1.0304545339535169</v>
+      </c>
+      <c r="O3" s="148">
+        <f>E3^alpha * (M3*D3)^beta</f>
+        <v>0.98204541963722647</v>
+      </c>
+      <c r="P3" s="148">
+        <f>((1-gamma_E)^1 * O3^phi + gamma_E^1 * ($N3*F3)^phi)^invPhi</f>
+        <v>0.98396167802821932</v>
+      </c>
+      <c r="Q3" s="148">
+        <f>((1-gamma_E)^1 * P3^phi + gamma_E^1 * ($N3*G3)^phi)^invPhi</f>
+        <v>0.98521092721352754</v>
+      </c>
+      <c r="R3" s="148">
+        <f>((1-gamma_E)^1 * Q3^phi + gamma_E^1 * ($N3*H3)^phi)^invPhi</f>
+        <v>0.9893981553015504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="148">
+        <f>UKData!A4</f>
+        <v>1982</v>
+      </c>
+      <c r="B4" s="148">
+        <f>UKData!B4</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="148">
+        <f>UKData!C4</f>
+        <v>1.0074198667253054</v>
+      </c>
+      <c r="D4" s="148">
+        <f>UKData!D4</f>
+        <v>0.93335655404620921</v>
+      </c>
+      <c r="E4" s="148">
+        <f>UKData!E4</f>
+        <v>1.0407303065950715</v>
+      </c>
+      <c r="F4" s="148">
+        <f>UKData!F4</f>
+        <v>0.94893665225329593</v>
+      </c>
+      <c r="G4" s="148">
+        <f>UKData!G4</f>
+        <v>0.94731929034470241</v>
+      </c>
+      <c r="H4" s="148">
+        <f>UKData!H4</f>
+        <v>0.90686470029314881</v>
+      </c>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" s="149">
+        <v>1.4E-2</v>
+      </c>
+      <c r="L4" s="148"/>
+      <c r="M4" s="148">
+        <f>EXP(lambda_L*B4)</f>
+        <v>1.028395684421425</v>
+      </c>
+      <c r="N4" s="148">
+        <f>EXP(lambda_E*B4)</f>
+        <v>1.0618365465453596</v>
+      </c>
+      <c r="O4" s="148">
+        <f>E4^alpha * (M4*D4)^beta</f>
+        <v>0.9826427078018557</v>
+      </c>
+      <c r="P4" s="148">
+        <f>((1-gamma_E)^1 * O4^phi + gamma_E^1 * ($N4*F4)^phi)^invPhi</f>
+        <v>0.98892876268345242</v>
+      </c>
+      <c r="Q4" s="148">
+        <f>((1-gamma_E)^1 * P4^phi + gamma_E^1 * ($N4*G4)^phi)^invPhi</f>
+        <v>0.99313521416933348</v>
+      </c>
+      <c r="R4" s="148">
+        <f>((1-gamma_E)^1 * Q4^phi + gamma_E^1 * ($N4*H4)^phi)^invPhi</f>
+        <v>0.98630130616264811</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="148">
+        <f>UKData!A5</f>
+        <v>1983</v>
+      </c>
+      <c r="B5" s="148">
+        <f>UKData!B5</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="148">
+        <f>UKData!C5</f>
+        <v>1.0439302403933943</v>
+      </c>
+      <c r="D5" s="148">
+        <f>UKData!D5</f>
+        <v>0.92337164750957856</v>
+      </c>
+      <c r="E5" s="148">
+        <f>UKData!E5</f>
+        <v>1.0662694571380202</v>
+      </c>
+      <c r="F5" s="148">
+        <f>UKData!F5</f>
+        <v>0.95305457275026917</v>
+      </c>
+      <c r="G5" s="148">
+        <f>UKData!G5</f>
+        <v>0.95085358384391472</v>
+      </c>
+      <c r="H5" s="148">
+        <f>UKData!H5</f>
+        <v>0.95209899535744169</v>
+      </c>
+      <c r="I5" s="148"/>
+      <c r="J5" s="148" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="149">
+        <v>0.03</v>
+      </c>
+      <c r="L5" s="148"/>
+      <c r="M5" s="148">
+        <f>EXP(lambda_L*B5)</f>
+        <v>1.0428944787507632</v>
+      </c>
+      <c r="N5" s="148">
+        <f>EXP(lambda_E*B5)</f>
+        <v>1.0941742837052104</v>
+      </c>
+      <c r="O5" s="148">
+        <f>E5^alpha * (M5*D5)^beta</f>
+        <v>0.99185782182387028</v>
+      </c>
+      <c r="P5" s="148">
+        <f>((1-gamma_E)^1 * O5^phi + gamma_E^1 * ($N5*F5)^phi)^invPhi</f>
+        <v>1.0053039023538035</v>
+      </c>
+      <c r="Q5" s="148">
+        <f>((1-gamma_E)^1 * P5^phi + gamma_E^1 * ($N5*G5)^phi)^invPhi</f>
+        <v>1.0142937165247956</v>
+      </c>
+      <c r="R5" s="148">
+        <f>((1-gamma_E)^1 * Q5^phi + gamma_E^1 * ($N5*H5)^phi)^invPhi</f>
+        <v>1.0212292932009819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="148">
+        <f>UKData!A6</f>
+        <v>1984</v>
+      </c>
+      <c r="B6" s="148">
+        <f>UKData!B6</f>
+        <v>4</v>
+      </c>
+      <c r="C6" s="148">
+        <f>UKData!C6</f>
+        <v>1.0718119648887277</v>
+      </c>
+      <c r="D6" s="148">
+        <f>UKData!D6</f>
+        <v>0.9465923603854639</v>
+      </c>
+      <c r="E6" s="148">
+        <f>UKData!E6</f>
+        <v>1.098967929092642</v>
+      </c>
+      <c r="F6" s="148">
+        <f>UKData!F6</f>
+        <v>0.93739330842206692</v>
+      </c>
+      <c r="G6" s="148">
+        <f>UKData!G6</f>
+        <v>0.93311273919560012</v>
+      </c>
+      <c r="H6" s="148">
+        <f>UKData!H6</f>
+        <v>1.0316867837963388</v>
+      </c>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148" t="s">
+        <v>154</v>
+      </c>
+      <c r="K6" s="148">
+        <f>(K1-1)/K1</f>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="L6" s="148" t="s">
+        <v>155</v>
+      </c>
+      <c r="M6" s="148">
+        <f>EXP(lambda_L*B6)</f>
+        <v>1.0575976837366112</v>
+      </c>
+      <c r="N6" s="148">
+        <f>EXP(lambda_E*B6)</f>
+        <v>1.1274968515793757</v>
+      </c>
+      <c r="O6" s="148">
+        <f>E6^alpha * (M6*D6)^beta</f>
+        <v>1.0285583413397639</v>
+      </c>
+      <c r="P6" s="148">
+        <f>((1-gamma_E)^1 * O6^phi + gamma_E^1 * ($N6*F6)^phi)^invPhi</f>
+        <v>1.0357227589991538</v>
+      </c>
+      <c r="Q6" s="148">
+        <f>((1-gamma_E)^1 * P6^phi + gamma_E^1 * ($N6*G6)^phi)^invPhi</f>
+        <v>1.0397675370466226</v>
+      </c>
+      <c r="R6" s="148">
+        <f>((1-gamma_E)^1 * Q6^phi + gamma_E^1 * ($N6*H6)^phi)^invPhi</f>
+        <v>1.0763430375521577</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="148">
+        <f>UKData!A7</f>
+        <v>1985</v>
+      </c>
+      <c r="B7" s="148">
+        <f>UKData!B7</f>
+        <v>5</v>
+      </c>
+      <c r="C7" s="148">
+        <f>UKData!C7</f>
+        <v>1.1103961291528321</v>
+      </c>
+      <c r="D7" s="148">
+        <f>UKData!D7</f>
+        <v>0.95982816672471849</v>
+      </c>
+      <c r="E7" s="148">
+        <f>UKData!E7</f>
+        <v>1.1338535752888379</v>
+      </c>
+      <c r="F7" s="148">
+        <f>UKData!F7</f>
+        <v>0.98238997632080727</v>
+      </c>
+      <c r="G7" s="148">
+        <f>UKData!G7</f>
+        <v>0.97887658997674099</v>
+      </c>
+      <c r="H7" s="148">
+        <f>UKData!H7</f>
+        <v>1.0175304105451042</v>
+      </c>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148" t="s">
+        <v>156</v>
+      </c>
+      <c r="K7" s="148">
+        <f>1/K6</f>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="L7" s="148" t="s">
+        <v>157</v>
+      </c>
+      <c r="M7" s="148">
+        <f>EXP(lambda_L*B7)</f>
+        <v>1.0725081812542165</v>
+      </c>
+      <c r="N7" s="148">
+        <f>EXP(lambda_E*B7)</f>
+        <v>1.1618342427282831</v>
+      </c>
+      <c r="O7" s="148">
+        <f>E7^alpha * (M7*D7)^beta</f>
+        <v>1.0586766546200896</v>
+      </c>
+      <c r="P7" s="148">
+        <f>((1-gamma_E)^1 * O7^phi + gamma_E^1 * ($N7*F7)^phi)^invPhi</f>
+        <v>1.0815557864358083</v>
+      </c>
+      <c r="Q7" s="148">
+        <f>((1-gamma_E)^1 * P7^phi + gamma_E^1 * ($N7*G7)^phi)^invPhi</f>
+        <v>1.0962694466191876</v>
+      </c>
+      <c r="R7" s="148">
+        <f>((1-gamma_E)^1 * Q7^phi + gamma_E^1 * ($N7*H7)^phi)^invPhi</f>
+        <v>1.1200546602893982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="148">
+        <f>UKData!A8</f>
+        <v>1986</v>
+      </c>
+      <c r="B8" s="148">
+        <f>UKData!B8</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="148">
+        <f>UKData!C8</f>
+        <v>1.1549496212053019</v>
+      </c>
+      <c r="D8" s="148">
+        <f>UKData!D8</f>
+        <v>0.96296296296296313</v>
+      </c>
+      <c r="E8" s="148">
+        <f>UKData!E8</f>
+        <v>1.1687497635780608</v>
+      </c>
+      <c r="F8" s="148">
+        <f>UKData!F8</f>
+        <v>1.005311255519197</v>
+      </c>
+      <c r="G8" s="148">
+        <f>UKData!G8</f>
+        <v>1.0023979637595191</v>
+      </c>
+      <c r="H8" s="148">
+        <f>UKData!H8</f>
+        <v>1.0315265146665604</v>
+      </c>
+      <c r="I8" s="148"/>
+      <c r="J8" s="148" t="s">
+        <v>158</v>
+      </c>
+      <c r="K8" s="148">
+        <f>1/K1</f>
+        <v>-5</v>
+      </c>
+      <c r="L8" s="148" t="s">
+        <v>159</v>
+      </c>
+      <c r="M8" s="148">
+        <f>EXP(lambda_L*B8)</f>
+        <v>1.0876288938088261</v>
+      </c>
+      <c r="N8" s="148">
+        <f>EXP(lambda_E*B8)</f>
+        <v>1.1972173631218102</v>
+      </c>
+      <c r="O8" s="148">
+        <f>E8^alpha * (M8*D8)^beta</f>
+        <v>1.0811933674195449</v>
+      </c>
+      <c r="P8" s="148">
+        <f>((1-gamma_E)^1 * O8^phi + gamma_E^1 * ($N8*F8)^phi)^invPhi</f>
+        <v>1.1171222599763235</v>
+      </c>
+      <c r="Q8" s="148">
+        <f>((1-gamma_E)^1 * P8^phi + gamma_E^1 * ($N8*G8)^phi)^invPhi</f>
+        <v>1.139922667202862</v>
+      </c>
+      <c r="R8" s="148">
+        <f>((1-gamma_E)^1 * Q8^phi + gamma_E^1 * ($N8*H8)^phi)^invPhi</f>
+        <v>1.1664560642764588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="148">
+        <f>UKData!A9</f>
+        <v>1987</v>
+      </c>
+      <c r="B9" s="148">
+        <f>UKData!B9</f>
+        <v>7</v>
+      </c>
+      <c r="C9" s="148">
+        <f>UKData!C9</f>
+        <v>1.2076422484039357</v>
+      </c>
+      <c r="D9" s="148">
+        <f>UKData!D9</f>
+        <v>0.98479043306629521</v>
+      </c>
+      <c r="E9" s="148">
+        <f>UKData!E9</f>
+        <v>1.2120318768088216</v>
+      </c>
+      <c r="F9" s="148">
+        <f>UKData!F9</f>
+        <v>1.0172650596334927</v>
+      </c>
+      <c r="G9" s="148">
+        <f>UKData!G9</f>
+        <v>1.0144579719009115</v>
+      </c>
+      <c r="H9" s="148">
+        <f>UKData!H9</f>
+        <v>1.1298445922656668</v>
+      </c>
+      <c r="I9" s="148"/>
+      <c r="J9" s="148" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="148">
+        <f>1-K3</f>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="L9" s="148"/>
+      <c r="M9" s="148">
+        <f>EXP(lambda_L*B9)</f>
+        <v>1.1029627851085078</v>
+      </c>
+      <c r="N9" s="148">
+        <f>EXP(lambda_E*B9)</f>
+        <v>1.2336780599567432</v>
+      </c>
+      <c r="O9" s="148">
+        <f>E9^alpha * (M9*D9)^beta</f>
+        <v>1.1212730788140743</v>
+      </c>
+      <c r="P9" s="148">
+        <f>((1-gamma_E)^1 * O9^phi + gamma_E^1 * ($N9*F9)^phi)^invPhi</f>
+        <v>1.1609178161825917</v>
+      </c>
+      <c r="Q9" s="148">
+        <f>((1-gamma_E)^1 * P9^phi + gamma_E^1 * ($N9*G9)^phi)^invPhi</f>
+        <v>1.1859790314050227</v>
+      </c>
+      <c r="R9" s="148">
+        <f>((1-gamma_E)^1 * Q9^phi + gamma_E^1 * ($N9*H9)^phi)^invPhi</f>
+        <v>1.2532675172290602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="148">
+        <f>UKData!A10</f>
+        <v>1988</v>
+      </c>
+      <c r="B10" s="148">
+        <f>UKData!B10</f>
+        <v>8</v>
+      </c>
+      <c r="C10" s="148">
+        <f>UKData!C10</f>
+        <v>1.2684097138100394</v>
+      </c>
+      <c r="D10" s="148">
+        <f>UKData!D10</f>
+        <v>1.0213630558458144</v>
+      </c>
+      <c r="E10" s="148">
+        <f>UKData!E10</f>
+        <v>1.2708548955309587</v>
+      </c>
+      <c r="F10" s="148">
+        <f>UKData!F10</f>
+        <v>1.0198761958893883</v>
+      </c>
+      <c r="G10" s="148">
+        <f>UKData!G10</f>
+        <v>1.0161118564960776</v>
+      </c>
+      <c r="H10" s="148">
+        <f>UKData!H10</f>
+        <v>1.1561078512777034</v>
+      </c>
+      <c r="I10" s="148"/>
+      <c r="J10" s="148"/>
+      <c r="K10" s="148"/>
+      <c r="L10" s="148"/>
+      <c r="M10" s="148">
+        <f>EXP(lambda_L*B10)</f>
+        <v>1.1185128606450452</v>
+      </c>
+      <c r="N10" s="148">
+        <f>EXP(lambda_E*B10)</f>
+        <v>1.2712491503214047</v>
+      </c>
+      <c r="O10" s="148">
+        <f>E10^alpha * (M10*D10)^beta</f>
+        <v>1.1782591748038536</v>
+      </c>
+      <c r="P10" s="148">
+        <f>((1-gamma_E)^1 * O10^phi + gamma_E^1 * ($N10*F10)^phi)^invPhi</f>
+        <v>1.2122433260804284</v>
+      </c>
+      <c r="Q10" s="148">
+        <f>((1-gamma_E)^1 * P10^phi + gamma_E^1 * ($N10*G10)^phi)^invPhi</f>
+        <v>1.2337574847873471</v>
+      </c>
+      <c r="R10" s="148">
+        <f>((1-gamma_E)^1 * Q10^phi + gamma_E^1 * ($N10*H10)^phi)^invPhi</f>
+        <v>1.3119437788212827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="148">
+        <f>UKData!A11</f>
+        <v>1989</v>
+      </c>
+      <c r="B11" s="148">
+        <f>UKData!B11</f>
+        <v>9</v>
+      </c>
+      <c r="C11" s="148">
+        <f>UKData!C11</f>
+        <v>1.2973501945625365</v>
+      </c>
+      <c r="D11" s="148">
+        <f>UKData!D11</f>
+        <v>1.0502728433762918</v>
+      </c>
+      <c r="E11" s="148">
+        <f>UKData!E11</f>
+        <v>1.3343226364162342</v>
+      </c>
+      <c r="F11" s="148">
+        <f>UKData!F11</f>
+        <v>1.0446640562684766</v>
+      </c>
+      <c r="G11" s="148">
+        <f>UKData!G11</f>
+        <v>1.0404417284802319</v>
+      </c>
+      <c r="H11" s="148">
+        <f>UKData!H11</f>
+        <v>1.1731038114886863</v>
+      </c>
+      <c r="I11" s="148"/>
+      <c r="J11" s="148"/>
+      <c r="K11" s="148"/>
+      <c r="L11" s="148"/>
+      <c r="M11" s="148">
+        <f>EXP(lambda_L*B11)</f>
+        <v>1.1342821682830251</v>
+      </c>
+      <c r="N11" s="148">
+        <f>EXP(lambda_E*B11)</f>
+        <v>1.3099644507332473</v>
+      </c>
+      <c r="O11" s="148">
+        <f>E11^alpha * (M11*D11)^beta</f>
+        <v>1.2311249948574692</v>
+      </c>
+      <c r="P11" s="148">
+        <f>((1-gamma_E)^1 * O11^phi + gamma_E^1 * ($N11*F11)^phi)^invPhi</f>
+        <v>1.2713389286155852</v>
+      </c>
+      <c r="Q11" s="148">
+        <f>((1-gamma_E)^1 * P11^phi + gamma_E^1 * ($N11*G11)^phi)^invPhi</f>
+        <v>1.2964157128401159</v>
+      </c>
+      <c r="R11" s="148">
+        <f>((1-gamma_E)^1 * Q11^phi + gamma_E^1 * ($N11*H11)^phi)^invPhi</f>
+        <v>1.3753681651237346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="148">
+        <f>UKData!A12</f>
+        <v>1990</v>
+      </c>
+      <c r="B12" s="148">
+        <f>UKData!B12</f>
+        <v>10</v>
+      </c>
+      <c r="C12" s="148">
+        <f>UKData!C12</f>
+        <v>1.3074619597878372</v>
+      </c>
+      <c r="D12" s="148">
+        <f>UKData!D12</f>
+        <v>1.0474863578311855</v>
+      </c>
+      <c r="E12" s="148">
+        <f>UKData!E12</f>
+        <v>1.3899793064915109</v>
+      </c>
+      <c r="F12" s="148">
+        <f>UKData!F12</f>
+        <v>1.0495614888952707</v>
+      </c>
+      <c r="G12" s="148">
+        <f>UKData!G12</f>
+        <v>1.0448086552770917</v>
+      </c>
+      <c r="H12" s="148">
+        <f>UKData!H12</f>
+        <v>1.2083466946064321</v>
+      </c>
+      <c r="I12" s="148"/>
+      <c r="J12" s="148"/>
+      <c r="K12" s="148"/>
+      <c r="L12" s="148"/>
+      <c r="M12" s="148">
+        <f>EXP(lambda_L*B12)</f>
+        <v>1.1502737988572274</v>
+      </c>
+      <c r="N12" s="148">
+        <f>EXP(lambda_E*B12)</f>
+        <v>1.3498588075760032</v>
+      </c>
+      <c r="O12" s="148">
+        <f>E12^alpha * (M12*D12)^beta</f>
+        <v>1.2558756359820333</v>
+      </c>
+      <c r="P12" s="148">
+        <f>((1-gamma_E)^1 * O12^phi + gamma_E^1 * ($N12*F12)^phi)^invPhi</f>
+        <v>1.3042708170641446</v>
+      </c>
+      <c r="Q12" s="148">
+        <f>((1-gamma_E)^1 * P12^phi + gamma_E^1 * ($N12*G12)^phi)^invPhi</f>
+        <v>1.3337806682474582</v>
+      </c>
+      <c r="R12" s="148">
+        <f>((1-gamma_E)^1 * Q12^phi + gamma_E^1 * ($N12*H12)^phi)^invPhi</f>
+        <v>1.436811067725533</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="148">
+        <f>UKData!A13</f>
+        <v>1991</v>
+      </c>
+      <c r="B13" s="148">
+        <f>UKData!B13</f>
+        <v>11</v>
+      </c>
+      <c r="C13" s="148">
+        <f>UKData!C13</f>
+        <v>1.2892539240421685</v>
+      </c>
+      <c r="D13" s="148">
+        <f>UKData!D13</f>
+        <v>1.0051085568326947</v>
+      </c>
+      <c r="E13" s="148">
+        <f>UKData!E13</f>
+        <v>1.4296355598440513</v>
+      </c>
+      <c r="F13" s="148">
+        <f>UKData!F13</f>
+        <v>1.0725814047203326</v>
+      </c>
+      <c r="G13" s="148">
+        <f>UKData!G13</f>
+        <v>1.0676384177349121</v>
+      </c>
+      <c r="H13" s="148">
+        <f>UKData!H13</f>
+        <v>1.1602740547707242</v>
+      </c>
+      <c r="I13" s="148"/>
+      <c r="J13" s="148"/>
+      <c r="K13" s="148"/>
+      <c r="L13" s="148"/>
+      <c r="M13" s="148">
+        <f>EXP(lambda_L*B13)</f>
+        <v>1.1664908867784396</v>
+      </c>
+      <c r="N13" s="148">
+        <f>EXP(lambda_E*B13)</f>
+        <v>1.3909681284637803</v>
+      </c>
+      <c r="O13" s="148">
+        <f>E13^alpha * (M13*D13)^beta</f>
+        <v>1.2418590791082993</v>
+      </c>
+      <c r="P13" s="148">
+        <f>((1-gamma_E)^1 * O13^phi + gamma_E^1 * ($N13*F13)^phi)^invPhi</f>
+        <v>1.3259424523301935</v>
+      </c>
+      <c r="Q13" s="148">
+        <f>((1-gamma_E)^1 * P13^phi + gamma_E^1 * ($N13*G13)^phi)^invPhi</f>
+        <v>1.3731778324885437</v>
+      </c>
+      <c r="R13" s="148">
+        <f>((1-gamma_E)^1 * Q13^phi + gamma_E^1 * ($N13*H13)^phi)^invPhi</f>
+        <v>1.4510986356240456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="148">
+        <f>UKData!A14</f>
+        <v>1992</v>
+      </c>
+      <c r="B14" s="148">
+        <f>UKData!B14</f>
+        <v>12</v>
+      </c>
+      <c r="C14" s="148">
+        <f>UKData!C14</f>
+        <v>1.2911442540397766</v>
+      </c>
+      <c r="D14" s="148">
+        <f>UKData!D14</f>
+        <v>0.97735980494601193</v>
+      </c>
+      <c r="E14" s="148">
+        <f>UKData!E14</f>
+        <v>1.4652783763688442</v>
+      </c>
+      <c r="F14" s="148">
+        <f>UKData!F14</f>
+        <v>1.0473870001799341</v>
+      </c>
+      <c r="G14" s="148">
+        <f>UKData!G14</f>
+        <v>1.0409692647668638</v>
+      </c>
+      <c r="H14" s="148">
+        <f>UKData!H14</f>
+        <v>1.2361844637663908</v>
+      </c>
+      <c r="I14" s="148"/>
+      <c r="J14" s="148"/>
+      <c r="K14" s="148"/>
+      <c r="L14" s="148"/>
+      <c r="M14" s="148">
+        <f>EXP(lambda_L*B14)</f>
+        <v>1.1829366106478107</v>
+      </c>
+      <c r="N14" s="148">
+        <f>EXP(lambda_E*B14)</f>
+        <v>1.4333294145603401</v>
+      </c>
+      <c r="O14" s="148">
+        <f>E14^alpha * (M14*D14)^beta</f>
+        <v>1.2383920725712281</v>
+      </c>
+      <c r="P14" s="148">
+        <f>((1-gamma_E)^1 * O14^phi + gamma_E^1 * ($N14*F14)^phi)^invPhi</f>
+        <v>1.3281469370774213</v>
+      </c>
+      <c r="Q14" s="148">
+        <f>((1-gamma_E)^1 * P14^phi + gamma_E^1 * ($N14*G14)^phi)^invPhi</f>
+        <v>1.3770774072995977</v>
+      </c>
+      <c r="R14" s="148">
+        <f>((1-gamma_E)^1 * Q14^phi + gamma_E^1 * ($N14*H14)^phi)^invPhi</f>
+        <v>1.5256282533063135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="148">
+        <f>UKData!A15</f>
+        <v>1993</v>
+      </c>
+      <c r="B15" s="148">
+        <f>UKData!B15</f>
+        <v>13</v>
+      </c>
+      <c r="C15" s="148">
+        <f>UKData!C15</f>
+        <v>1.3198395491327199</v>
+      </c>
+      <c r="D15" s="148">
+        <f>UKData!D15</f>
+        <v>0.96632996632996637</v>
+      </c>
+      <c r="E15" s="148">
+        <f>UKData!E15</f>
+        <v>1.4980934314698839</v>
+      </c>
+      <c r="F15" s="148">
+        <f>UKData!F15</f>
+        <v>1.0593407554886922</v>
+      </c>
+      <c r="G15" s="148">
+        <f>UKData!G15</f>
+        <v>1.05088712450417</v>
+      </c>
+      <c r="H15" s="148">
+        <f>UKData!H15</f>
+        <v>1.2454504444578405</v>
+      </c>
+      <c r="I15" s="148"/>
+      <c r="J15" s="148"/>
+      <c r="K15" s="148"/>
+      <c r="L15" s="148"/>
+      <c r="M15" s="148">
+        <f>EXP(lambda_L*B15)</f>
+        <v>1.1996141938798683</v>
+      </c>
+      <c r="N15" s="148">
+        <f>EXP(lambda_E*B15)</f>
+        <v>1.4769807938826427</v>
+      </c>
+      <c r="O15" s="148">
+        <f>E15^alpha * (M15*D15)^beta</f>
+        <v>1.2487194650723561</v>
+      </c>
+      <c r="P15" s="148">
+        <f>((1-gamma_E)^1 * O15^phi + gamma_E^1 * ($N15*F15)^phi)^invPhi</f>
+        <v>1.3626715415978905</v>
+      </c>
+      <c r="Q15" s="148">
+        <f>((1-gamma_E)^1 * P15^phi + gamma_E^1 * ($N15*G15)^phi)^invPhi</f>
+        <v>1.4206706465137608</v>
+      </c>
+      <c r="R15" s="148">
+        <f>((1-gamma_E)^1 * Q15^phi + gamma_E^1 * ($N15*H15)^phi)^invPhi</f>
+        <v>1.5798223829201554</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="148">
+        <f>UKData!A16</f>
+        <v>1994</v>
+      </c>
+      <c r="B16" s="148">
+        <f>UKData!B16</f>
+        <v>14</v>
+      </c>
+      <c r="C16" s="148">
+        <f>UKData!C16</f>
+        <v>1.3763325540544364</v>
+      </c>
+      <c r="D16" s="148">
+        <f>UKData!D16</f>
+        <v>0.97979797979797989</v>
+      </c>
+      <c r="E16" s="148">
+        <f>UKData!E16</f>
+        <v>1.5348289049307851</v>
+      </c>
+      <c r="F16" s="148">
+        <f>UKData!F16</f>
+        <v>1.0655408988581594</v>
+      </c>
+      <c r="G16" s="148">
+        <f>UKData!G16</f>
+        <v>1.0562790147853107</v>
+      </c>
+      <c r="H16" s="148">
+        <f>UKData!H16</f>
+        <v>1.4084465168078506</v>
+      </c>
+      <c r="I16" s="148"/>
+      <c r="J16" s="148"/>
+      <c r="K16" s="148"/>
+      <c r="L16" s="148"/>
+      <c r="M16" s="148">
+        <f>EXP(lambda_L*B16)</f>
+        <v>1.2165269053343162</v>
+      </c>
+      <c r="N16" s="148">
+        <f>EXP(lambda_E*B16)</f>
+        <v>1.5219615556186337</v>
+      </c>
+      <c r="O16" s="148">
+        <f>E16^alpha * (M16*D16)^beta</f>
+        <v>1.2826281122824086</v>
+      </c>
+      <c r="P16" s="148">
+        <f>((1-gamma_E)^1 * O16^phi + gamma_E^1 * ($N16*F16)^phi)^invPhi</f>
+        <v>1.4067381840208246</v>
+      </c>
+      <c r="Q16" s="148">
+        <f>((1-gamma_E)^1 * P16^phi + gamma_E^1 * ($N16*G16)^phi)^invPhi</f>
+        <v>1.4685959004696909</v>
+      </c>
+      <c r="R16" s="148">
+        <f>((1-gamma_E)^1 * Q16^phi + gamma_E^1 * ($N16*H16)^phi)^invPhi</f>
+        <v>1.771532937025222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="148">
+        <f>UKData!A17</f>
+        <v>1995</v>
+      </c>
+      <c r="B17" s="148">
+        <f>UKData!B17</f>
+        <v>15</v>
+      </c>
+      <c r="C17" s="148">
+        <f>UKData!C17</f>
+        <v>1.4183407446271334</v>
+      </c>
+      <c r="D17" s="148">
+        <f>UKData!D17</f>
+        <v>0.99314988970161389</v>
+      </c>
+      <c r="E17" s="148">
+        <f>UKData!E17</f>
+        <v>1.5731512734538315</v>
+      </c>
+      <c r="F17" s="148">
+        <f>UKData!F17</f>
+        <v>1.0623232474418691</v>
+      </c>
+      <c r="G17" s="148">
+        <f>UKData!G17</f>
+        <v>1.0518946557261688</v>
+      </c>
+      <c r="H17" s="148">
+        <f>UKData!H17</f>
+        <v>1.4071206040748148</v>
+      </c>
+      <c r="I17" s="148"/>
+      <c r="J17" s="148"/>
+      <c r="K17" s="148"/>
+      <c r="L17" s="148"/>
+      <c r="M17" s="148">
+        <f>EXP(lambda_L*B17)</f>
+        <v>1.2336780599567432</v>
+      </c>
+      <c r="N17" s="148">
+        <f>EXP(lambda_E*B17)</f>
+        <v>1.5683121854901687</v>
+      </c>
+      <c r="O17" s="148">
+        <f>E17^alpha * (M17*D17)^beta</f>
+        <v>1.3173381080974642</v>
+      </c>
+      <c r="P17" s="148">
+        <f>((1-gamma_E)^1 * O17^phi + gamma_E^1 * ($N17*F17)^phi)^invPhi</f>
+        <v>1.445029721599703</v>
+      </c>
+      <c r="Q17" s="148">
+        <f>((1-gamma_E)^1 * P17^phi + gamma_E^1 * ($N17*G17)^phi)^invPhi</f>
+        <v>1.507939795821793</v>
+      </c>
+      <c r="R17" s="148">
+        <f>((1-gamma_E)^1 * Q17^phi + gamma_E^1 * ($N17*H17)^phi)^invPhi</f>
+        <v>1.8225940142907644</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="148">
+        <f>UKData!A18</f>
+        <v>1996</v>
+      </c>
+      <c r="B18" s="148">
+        <f>UKData!B18</f>
+        <v>16</v>
+      </c>
+      <c r="C18" s="148">
+        <f>UKData!C18</f>
+        <v>1.4592636028746733</v>
+      </c>
+      <c r="D18" s="148">
+        <f>UKData!D18</f>
+        <v>1.0020898641588296</v>
+      </c>
+      <c r="E18" s="148">
+        <f>UKData!E18</f>
+        <v>1.6167099615957752</v>
+      </c>
+      <c r="F18" s="148">
+        <f>UKData!F18</f>
+        <v>1.1283147425331463</v>
+      </c>
+      <c r="G18" s="148">
+        <f>UKData!G18</f>
+        <v>1.1167318059906117</v>
+      </c>
+      <c r="H18" s="148">
+        <f>UKData!H18</f>
+        <v>1.4547425302102142</v>
+      </c>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
+      <c r="K18" s="148"/>
+      <c r="L18" s="148"/>
+      <c r="M18" s="148">
+        <f>EXP(lambda_L*B18)</f>
+        <v>1.2510710194283623</v>
+      </c>
+      <c r="N18" s="148">
+        <f>EXP(lambda_E*B18)</f>
+        <v>1.6160744021928934</v>
+      </c>
+      <c r="O18" s="148">
+        <f>E18^alpha * (M18*D18)^beta</f>
+        <v>1.3496378296973555</v>
+      </c>
+      <c r="P18" s="148">
+        <f>((1-gamma_E)^1 * O18^phi + gamma_E^1 * ($N18*F18)^phi)^invPhi</f>
+        <v>1.5414600854987146</v>
+      </c>
+      <c r="Q18" s="148">
+        <f>((1-gamma_E)^1 * P18^phi + gamma_E^1 * ($N18*G18)^phi)^invPhi</f>
+        <v>1.6261000022738106</v>
+      </c>
+      <c r="R18" s="148">
+        <f>((1-gamma_E)^1 * Q18^phi + gamma_E^1 * ($N18*H18)^phi)^invPhi</f>
+        <v>1.9475854648171409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="148">
+        <f>UKData!A19</f>
+        <v>1997</v>
+      </c>
+      <c r="B19" s="148">
+        <f>UKData!B19</f>
+        <v>17</v>
+      </c>
+      <c r="C19" s="148">
+        <f>UKData!C19</f>
+        <v>1.5092188950699679</v>
+      </c>
+      <c r="D19" s="148">
+        <f>UKData!D19</f>
+        <v>1.019040984558226</v>
+      </c>
+      <c r="E19" s="148">
+        <f>UKData!E19</f>
+        <v>1.6682756794533986</v>
+      </c>
+      <c r="F19" s="148">
+        <f>UKData!F19</f>
+        <v>1.096275554146263</v>
+      </c>
+      <c r="G19" s="148">
+        <f>UKData!G19</f>
+        <v>1.0838257585871125</v>
+      </c>
+      <c r="H19" s="148">
+        <f>UKData!H19</f>
+        <v>1.4218456927515315</v>
+      </c>
+      <c r="I19" s="148"/>
+      <c r="J19" s="148"/>
+      <c r="K19" s="148"/>
+      <c r="L19" s="148"/>
+      <c r="M19" s="148">
+        <f>EXP(lambda_L*B19)</f>
+        <v>1.2687091928249108</v>
+      </c>
+      <c r="N19" s="148">
+        <f>EXP(lambda_E*B19)</f>
+        <v>1.6652911949458864</v>
+      </c>
+      <c r="O19" s="148">
+        <f>E19^alpha * (M19*D19)^beta</f>
+        <v>1.3920691890611541</v>
+      </c>
+      <c r="P19" s="148">
+        <f>((1-gamma_E)^1 * O19^phi + gamma_E^1 * ($N19*F19)^phi)^invPhi</f>
+        <v>1.5600573168782552</v>
+      </c>
+      <c r="Q19" s="148">
+        <f>((1-gamma_E)^1 * P19^phi + gamma_E^1 * ($N19*G19)^phi)^invPhi</f>
+        <v>1.6371281514975111</v>
+      </c>
+      <c r="R19" s="148">
+        <f>((1-gamma_E)^1 * Q19^phi + gamma_E^1 * ($N19*H19)^phi)^invPhi</f>
+        <v>1.9613296621290588</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="148">
+        <f>UKData!A20</f>
+        <v>1998</v>
+      </c>
+      <c r="B20" s="148">
+        <f>UKData!B20</f>
+        <v>18</v>
+      </c>
+      <c r="C20" s="148">
+        <f>UKData!C20</f>
+        <v>1.5671581524660447</v>
+      </c>
+      <c r="D20" s="148">
+        <f>UKData!D20</f>
+        <v>1.0272843376291652</v>
+      </c>
+      <c r="E20" s="148">
+        <f>UKData!E20</f>
+        <v>1.7385418300949471</v>
+      </c>
+      <c r="F20" s="148">
+        <f>UKData!F20</f>
+        <v>1.1003800043912437</v>
+      </c>
+      <c r="G20" s="148">
+        <f>UKData!G20</f>
+        <v>1.0871942651170379</v>
+      </c>
+      <c r="H20" s="148">
+        <f>UKData!H20</f>
+        <v>1.4526665345862682</v>
+      </c>
+      <c r="I20" s="148"/>
+      <c r="J20" s="148"/>
+      <c r="K20" s="148"/>
+      <c r="L20" s="148"/>
+      <c r="M20" s="148">
+        <f>EXP(lambda_L*B20)</f>
+        <v>1.2865960372848406</v>
+      </c>
+      <c r="N20" s="148">
+        <f>EXP(lambda_E*B20)</f>
+        <v>1.7160068621848585</v>
+      </c>
+      <c r="O20" s="148">
+        <f>E20^alpha * (M20*D20)^beta</f>
+        <v>1.4310606300145228</v>
+      </c>
+      <c r="P20" s="148">
+        <f>((1-gamma_E)^1 * O20^phi + gamma_E^1 * ($N20*F20)^phi)^invPhi</f>
+        <v>1.6098499415345771</v>
+      </c>
+      <c r="Q20" s="148">
+        <f>((1-gamma_E)^1 * P20^phi + gamma_E^1 * ($N20*G20)^phi)^invPhi</f>
+        <v>1.690611160720098</v>
+      </c>
+      <c r="R20" s="148">
+        <f>((1-gamma_E)^1 * Q20^phi + gamma_E^1 * ($N20*H20)^phi)^invPhi</f>
+        <v>2.0550834858247278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="148">
+        <f>UKData!A21</f>
+        <v>1999</v>
+      </c>
+      <c r="B21" s="148">
+        <f>UKData!B21</f>
+        <v>19</v>
+      </c>
+      <c r="C21" s="148">
+        <f>UKData!C21</f>
+        <v>1.6244484394275687</v>
+      </c>
+      <c r="D21" s="148">
+        <f>UKData!D21</f>
+        <v>1.03645651921514</v>
+      </c>
+      <c r="E21" s="148">
+        <f>UKData!E21</f>
+        <v>1.8091242435273098</v>
+      </c>
+      <c r="F21" s="148">
+        <f>UKData!F21</f>
+        <v>1.1025514987028602</v>
+      </c>
+      <c r="G21" s="148">
+        <f>UKData!G21</f>
+        <v>1.0885389898154771</v>
+      </c>
+      <c r="H21" s="148">
+        <f>UKData!H21</f>
+        <v>1.4201251139109066</v>
+      </c>
+      <c r="I21" s="148"/>
+      <c r="J21" s="148"/>
+      <c r="K21" s="148"/>
+      <c r="L21" s="148"/>
+      <c r="M21" s="148">
+        <f>EXP(lambda_L*B21)</f>
+        <v>1.304735058686928</v>
+      </c>
+      <c r="N21" s="148">
+        <f>EXP(lambda_E*B21)</f>
+        <v>1.7682670514337351</v>
+      </c>
+      <c r="O21" s="148">
+        <f>E21^alpha * (M21*D21)^beta</f>
+        <v>1.4713905489081049</v>
+      </c>
+      <c r="P21" s="148">
+        <f>((1-gamma_E)^1 * O21^phi + gamma_E^1 * ($N21*F21)^phi)^invPhi</f>
+        <v>1.659568015985913</v>
+      </c>
+      <c r="Q21" s="148">
+        <f>((1-gamma_E)^1 * P21^phi + gamma_E^1 * ($N21*G21)^phi)^invPhi</f>
+        <v>1.7434436217168832</v>
+      </c>
+      <c r="R21" s="148">
+        <f>((1-gamma_E)^1 * Q21^phi + gamma_E^1 * ($N21*H21)^phi)^invPhi</f>
+        <v>2.0823208758887146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="148">
+        <f>UKData!A22</f>
+        <v>2000</v>
+      </c>
+      <c r="B22" s="148">
+        <f>UKData!B22</f>
+        <v>20</v>
+      </c>
+      <c r="C22" s="148">
+        <f>UKData!C22</f>
+        <v>1.6968605090774418</v>
+      </c>
+      <c r="D22" s="148">
+        <f>UKData!D22</f>
+        <v>1.038894694067108</v>
+      </c>
+      <c r="E22" s="148">
+        <f>UKData!E22</f>
+        <v>1.8797072770827921</v>
+      </c>
+      <c r="F22" s="148">
+        <f>UKData!F22</f>
+        <v>1.0955263602376164</v>
+      </c>
+      <c r="G22" s="148">
+        <f>UKData!G22</f>
+        <v>1.0814970746755368</v>
+      </c>
+      <c r="H22" s="148">
+        <f>UKData!H22</f>
+        <v>1.49834855259282</v>
+      </c>
+      <c r="I22" s="148"/>
+      <c r="J22" s="148"/>
+      <c r="K22" s="148"/>
+      <c r="L22" s="148"/>
+      <c r="M22" s="148">
+        <f>EXP(lambda_L*B22)</f>
+        <v>1.3231298123374369</v>
+      </c>
+      <c r="N22" s="148">
+        <f>EXP(lambda_E*B22)</f>
+        <v>1.8221188003905089</v>
+      </c>
+      <c r="O22" s="148">
+        <f>E22^alpha * (M22*D22)^beta</f>
+        <v>1.5051843447627642</v>
+      </c>
+      <c r="P22" s="148">
+        <f>((1-gamma_E)^1 * O22^phi + gamma_E^1 * ($N22*F22)^phi)^invPhi</f>
+        <v>1.6986493023028608</v>
+      </c>
+      <c r="Q22" s="148">
+        <f>((1-gamma_E)^1 * P22^phi + gamma_E^1 * ($N22*G22)^phi)^invPhi</f>
+        <v>1.7846814916890481</v>
+      </c>
+      <c r="R22" s="148">
+        <f>((1-gamma_E)^1 * Q22^phi + gamma_E^1 * ($N22*H22)^phi)^invPhi</f>
+        <v>2.2329218897776486</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="148">
+        <f>UKData!A23</f>
+        <v>2001</v>
+      </c>
+      <c r="B23" s="148">
+        <f>UKData!B23</f>
+        <v>21</v>
+      </c>
+      <c r="C23" s="148">
+        <f>UKData!C23</f>
+        <v>1.7503229849553736</v>
+      </c>
+      <c r="D23" s="148">
+        <f>UKData!D23</f>
+        <v>1.0488796006037386</v>
+      </c>
+      <c r="E23" s="148">
+        <f>UKData!E23</f>
+        <v>1.9505854892430343</v>
+      </c>
+      <c r="F23" s="148">
+        <f>UKData!F23</f>
+        <v>1.1173156943676004</v>
+      </c>
+      <c r="G23" s="148">
+        <f>UKData!G23</f>
+        <v>1.1032292209563987</v>
+      </c>
+      <c r="H23" s="148" t="str">
+        <f>UKData!H23</f>
+        <v>NA</v>
+      </c>
+      <c r="I23" s="148"/>
+      <c r="J23" s="148"/>
+      <c r="K23" s="148"/>
+      <c r="L23" s="148"/>
+      <c r="M23" s="148">
+        <f>EXP(lambda_L*B23)</f>
+        <v>1.3417839036669714</v>
+      </c>
+      <c r="N23" s="148">
+        <f>EXP(lambda_E*B23)</f>
+        <v>1.8776105792643432</v>
+      </c>
+      <c r="O23" s="148">
+        <f>E23^alpha * (M23*D23)^beta</f>
+        <v>1.5470974869950189</v>
+      </c>
+      <c r="P23" s="148">
+        <f>((1-gamma_E)^1 * O23^phi + gamma_E^1 * ($N23*F23)^phi)^invPhi</f>
+        <v>1.7712579994817561</v>
+      </c>
+      <c r="Q23" s="148">
+        <f>((1-gamma_E)^1 * P23^phi + gamma_E^1 * ($N23*G23)^phi)^invPhi</f>
+        <v>1.867575183192886</v>
+      </c>
+      <c r="R23" s="148"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="148">
+        <f>UKData!A24</f>
+        <v>2002</v>
+      </c>
+      <c r="B24" s="148">
+        <f>UKData!B24</f>
+        <v>22</v>
+      </c>
+      <c r="C24" s="148">
+        <f>UKData!C24</f>
+        <v>1.7968379622842729</v>
+      </c>
+      <c r="D24" s="148">
+        <f>UKData!D24</f>
+        <v>1.0459770114942528</v>
+      </c>
+      <c r="E24" s="148">
+        <f>UKData!E24</f>
+        <v>2.0238604772591549</v>
+      </c>
+      <c r="F24" s="148">
+        <f>UKData!F24</f>
+        <v>1.1051073554598261</v>
+      </c>
+      <c r="G24" s="148">
+        <f>UKData!G24</f>
+        <v>1.090432185510017</v>
+      </c>
+      <c r="H24" s="148" t="str">
+        <f>UKData!H24</f>
+        <v>NA</v>
+      </c>
+      <c r="I24" s="148"/>
+      <c r="J24" s="148"/>
+      <c r="K24" s="148"/>
+      <c r="L24" s="148"/>
+      <c r="M24" s="148">
+        <f>EXP(lambda_L*B24)</f>
+        <v>1.3607009889371502</v>
+      </c>
+      <c r="N24" s="148">
+        <f>EXP(lambda_E*B24)</f>
+        <v>1.9347923344020315</v>
+      </c>
+      <c r="O24" s="148">
+        <f>E24^alpha * (M24*D24)^beta</f>
+        <v>1.576248192677399</v>
+      </c>
+      <c r="P24" s="148">
+        <f>((1-gamma_E)^1 * O24^phi + gamma_E^1 * ($N24*F24)^phi)^invPhi</f>
+        <v>1.8050468621415683</v>
+      </c>
+      <c r="Q24" s="148">
+        <f>((1-gamma_E)^1 * P24^phi + gamma_E^1 * ($N24*G24)^phi)^invPhi</f>
+        <v>1.9027223088273526</v>
+      </c>
+      <c r="R24" s="148"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="148">
+        <f>UKData!A25</f>
+        <v>2003</v>
+      </c>
+      <c r="B25" s="148">
+        <f>UKData!B25</f>
+        <v>23</v>
+      </c>
+      <c r="C25" s="148">
+        <f>UKData!C25</f>
+        <v>1.8601695896054997</v>
+      </c>
+      <c r="D25" s="148">
+        <f>UKData!D25</f>
+        <v>1.0499245326831534</v>
+      </c>
+      <c r="E25" s="148">
+        <f>UKData!E25</f>
+        <v>2.0943529728392276</v>
+      </c>
+      <c r="F25" s="148">
+        <f>UKData!F25</f>
+        <v>1.1121866035008878</v>
+      </c>
+      <c r="G25" s="148">
+        <f>UKData!G25</f>
+        <v>1.0982309355870383</v>
+      </c>
+      <c r="H25" s="148" t="str">
+        <f>UKData!H25</f>
+        <v>NA</v>
+      </c>
+      <c r="I25" s="148"/>
+      <c r="J25" s="148"/>
+      <c r="K25" s="148"/>
+      <c r="L25" s="148"/>
+      <c r="M25" s="148">
+        <f>EXP(lambda_L*B25)</f>
+        <v>1.3798847759572466</v>
+      </c>
+      <c r="N25" s="148">
+        <f>EXP(lambda_E*B25)</f>
+        <v>1.9937155332430823</v>
+      </c>
+      <c r="O25" s="148">
+        <f>E25^alpha * (M25*D25)^beta</f>
+        <v>1.6121858620418656</v>
+      </c>
+      <c r="P25" s="148">
+        <f>((1-gamma_E)^1 * O25^phi + gamma_E^1 * ($N25*F25)^phi)^invPhi</f>
+        <v>1.8634591840961265</v>
+      </c>
+      <c r="Q25" s="148">
+        <f>((1-gamma_E)^1 * P25^phi + gamma_E^1 * ($N25*G25)^phi)^invPhi</f>
+        <v>1.9689662606486766</v>
+      </c>
+      <c r="R25" s="148"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="148">
+        <f>UKData!A26</f>
+        <v>2004</v>
+      </c>
+      <c r="B26" s="148">
+        <f>UKData!B26</f>
+        <v>24</v>
+      </c>
+      <c r="C26" s="148">
+        <f>UKData!C26</f>
+        <v>1.9151434721890022</v>
+      </c>
+      <c r="D26" s="148">
+        <f>UKData!D26</f>
+        <v>1.0593289213978869</v>
+      </c>
+      <c r="E26" s="148">
+        <f>UKData!E26</f>
+        <v>2.1706895086950562</v>
+      </c>
+      <c r="F26" s="148">
+        <f>UKData!F26</f>
+        <v>1.1144255716268654</v>
+      </c>
+      <c r="G26" s="148">
+        <f>UKData!G26</f>
+        <v>1.1008020611638714</v>
+      </c>
+      <c r="H26" s="148" t="str">
+        <f>UKData!H26</f>
+        <v>NA</v>
+      </c>
+      <c r="I26" s="148"/>
+      <c r="J26" s="148"/>
+      <c r="K26" s="148"/>
+      <c r="L26" s="148"/>
+      <c r="M26" s="148">
+        <f>EXP(lambda_L*B26)</f>
+        <v>1.3993390248109305</v>
+      </c>
+      <c r="N26" s="148">
+        <f>EXP(lambda_E*B26)</f>
+        <v>2.0544332106438876</v>
+      </c>
+      <c r="O26" s="148">
+        <f>E26^alpha * (M26*D26)^beta</f>
+        <v>1.6557338039810936</v>
+      </c>
+      <c r="P26" s="148">
+        <f>((1-gamma_E)^1 * O26^phi + gamma_E^1 * ($N26*F26)^phi)^invPhi</f>
+        <v>1.9208287598332903</v>
+      </c>
+      <c r="Q26" s="148">
+        <f>((1-gamma_E)^1 * P26^phi + gamma_E^1 * ($N26*G26)^phi)^invPhi</f>
+        <v>2.0314482670938596</v>
+      </c>
+      <c r="R26" s="148"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="148">
+        <f>UKData!A27</f>
+        <v>2005</v>
+      </c>
+      <c r="B27" s="148">
+        <f>UKData!B27</f>
+        <v>25</v>
+      </c>
+      <c r="C27" s="148">
+        <f>UKData!C27</f>
+        <v>1.9550890169683908</v>
+      </c>
+      <c r="D27" s="148">
+        <f>UKData!D27</f>
+        <v>1.0719842099152443</v>
+      </c>
+      <c r="E27" s="148">
+        <f>UKData!E27</f>
+        <v>2.247073794031067</v>
+      </c>
+      <c r="F27" s="148">
+        <f>UKData!F27</f>
+        <v>1.1153375454227641</v>
+      </c>
+      <c r="G27" s="148">
+        <f>UKData!G27</f>
+        <v>1.101660059404304</v>
+      </c>
+      <c r="H27" s="148" t="str">
+        <f>UKData!H27</f>
+        <v>NA</v>
+      </c>
+      <c r="I27" s="148"/>
+      <c r="J27" s="148"/>
+      <c r="K27" s="148"/>
+      <c r="L27" s="148"/>
+      <c r="M27" s="148">
+        <f>EXP(lambda_L*B27)</f>
+        <v>1.4190675485932573</v>
+      </c>
+      <c r="N27" s="148">
+        <f>EXP(lambda_E*B27)</f>
+        <v>2.1170000166126748</v>
+      </c>
+      <c r="O27" s="148">
+        <f>E27^alpha * (M27*D27)^beta</f>
+        <v>1.7034326280795979</v>
+      </c>
+      <c r="P27" s="148">
+        <f>((1-gamma_E)^1 * O27^phi + gamma_E^1 * ($N27*F27)^phi)^invPhi</f>
+        <v>1.9794618118533096</v>
+      </c>
+      <c r="Q27" s="148">
+        <f>((1-gamma_E)^1 * P27^phi + gamma_E^1 * ($N27*G27)^phi)^invPhi</f>
+        <v>2.0941387532661095</v>
+      </c>
+      <c r="R27" s="148"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="148">
+        <f>UKData!A28</f>
+        <v>2006</v>
+      </c>
+      <c r="B28" s="148">
+        <f>UKData!B28</f>
+        <v>26</v>
+      </c>
+      <c r="C28" s="148">
+        <f>UKData!C28</f>
+        <v>2.0060610580875688</v>
+      </c>
+      <c r="D28" s="148">
+        <f>UKData!D28</f>
+        <v>1.0777893881342158</v>
+      </c>
+      <c r="E28" s="148">
+        <f>UKData!E28</f>
+        <v>2.3326861315045488</v>
+      </c>
+      <c r="F28" s="148">
+        <f>UKData!F28</f>
+        <v>1.1029046871711281</v>
+      </c>
+      <c r="G28" s="148">
+        <f>UKData!G28</f>
+        <v>1.0899275225463279</v>
+      </c>
+      <c r="H28" s="148" t="str">
+        <f>UKData!H28</f>
+        <v>NA</v>
+      </c>
+      <c r="I28" s="148"/>
+      <c r="J28" s="148"/>
+      <c r="K28" s="148"/>
+      <c r="L28" s="148"/>
+      <c r="M28" s="148">
+        <f>EXP(lambda_L*B28)</f>
+        <v>1.4390742141580464</v>
+      </c>
+      <c r="N28" s="148">
+        <f>EXP(lambda_E*B28)</f>
+        <v>2.1814722654982011</v>
+      </c>
+      <c r="O28" s="148">
+        <f>E28^alpha * (M28*D28)^beta</f>
+        <v>1.7458883472703948</v>
+      </c>
+      <c r="P28" s="148">
+        <f>((1-gamma_E)^1 * O28^phi + gamma_E^1 * ($N28*F28)^phi)^invPhi</f>
+        <v>2.0206836572844171</v>
+      </c>
+      <c r="Q28" s="148">
+        <f>((1-gamma_E)^1 * P28^phi + gamma_E^1 * ($N28*G28)^phi)^invPhi</f>
+        <v>2.1364617678108346</v>
+      </c>
+      <c r="R28" s="148"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="148">
+        <f>UKData!A29</f>
+        <v>2007</v>
+      </c>
+      <c r="B29" s="148">
+        <f>UKData!B29</f>
+        <v>27</v>
+      </c>
+      <c r="C29" s="148">
+        <f>UKData!C29</f>
+        <v>2.0755943394689758</v>
+      </c>
+      <c r="D29" s="148">
+        <f>UKData!D29</f>
+        <v>1.0868454661558111</v>
+      </c>
+      <c r="E29" s="148">
+        <f>UKData!E29</f>
+        <v>2.4319703233880055</v>
+      </c>
+      <c r="F29" s="148">
+        <f>UKData!F29</f>
+        <v>1.0609379497383971</v>
+      </c>
+      <c r="G29" s="148">
+        <f>UKData!G29</f>
+        <v>1.0478528164379208</v>
+      </c>
+      <c r="H29" s="148" t="str">
+        <f>UKData!H29</f>
+        <v>NA</v>
+      </c>
+      <c r="I29" s="148"/>
+      <c r="J29" s="148"/>
+      <c r="K29" s="148"/>
+      <c r="L29" s="148"/>
+      <c r="M29" s="148">
+        <f>EXP(lambda_L*B29)</f>
+        <v>1.4593629428757966</v>
+      </c>
+      <c r="N29" s="148">
+        <f>EXP(lambda_E*B29)</f>
+        <v>2.2479079866764713</v>
+      </c>
+      <c r="O29" s="148">
+        <f>E29^alpha * (M29*D29)^beta</f>
+        <v>1.7954073066123766</v>
+      </c>
+      <c r="P29" s="148">
+        <f>((1-gamma_E)^1 * O29^phi + gamma_E^1 * ($N29*F29)^phi)^invPhi</f>
+        <v>2.0282316174901402</v>
+      </c>
+      <c r="Q29" s="148">
+        <f>((1-gamma_E)^1 * P29^phi + gamma_E^1 * ($N29*G29)^phi)^invPhi</f>
+        <v>2.1319463819904176</v>
+      </c>
+      <c r="R29" s="148"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="148">
+        <f>UKData!A30</f>
+        <v>2008</v>
+      </c>
+      <c r="B30" s="148">
+        <f>UKData!B30</f>
+        <v>28</v>
+      </c>
+      <c r="C30" s="148">
+        <f>UKData!C30</f>
+        <v>2.0527029147088247</v>
+      </c>
+      <c r="D30" s="148">
+        <f>UKData!D30</f>
+        <v>1.0913735051666087</v>
+      </c>
+      <c r="E30" s="148">
+        <f>UKData!E30</f>
+        <v>2.511672267411972</v>
+      </c>
+      <c r="F30" s="148">
+        <f>UKData!F30</f>
+        <v>1.0494311120709716</v>
+      </c>
+      <c r="G30" s="148">
+        <f>UKData!G30</f>
+        <v>1.0360211715944556</v>
+      </c>
+      <c r="H30" s="148" t="str">
+        <f>UKData!H30</f>
+        <v>NA</v>
+      </c>
+      <c r="I30" s="148"/>
+      <c r="J30" s="148"/>
+      <c r="K30" s="148"/>
+      <c r="L30" s="148"/>
+      <c r="M30" s="148">
+        <f>EXP(lambda_L*B30)</f>
+        <v>1.4799377114022885</v>
+      </c>
+      <c r="N30" s="148">
+        <f>EXP(lambda_E*B30)</f>
+        <v>2.3163669767810915</v>
+      </c>
+      <c r="O30" s="148">
+        <f>E30^alpha * (M30*D30)^beta</f>
+        <v>1.8357909313118101</v>
+      </c>
+      <c r="P30" s="148">
+        <f>((1-gamma_E)^1 * O30^phi + gamma_E^1 * ($N30*F30)^phi)^invPhi</f>
+        <v>2.0697284323432674</v>
+      </c>
+      <c r="Q30" s="148">
+        <f>((1-gamma_E)^1 * P30^phi + gamma_E^1 * ($N30*G30)^phi)^invPhi</f>
+        <v>2.1740420478006035</v>
+      </c>
+      <c r="R30" s="148"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="148">
+        <f>UKData!A31</f>
+        <v>2009</v>
+      </c>
+      <c r="B31" s="148">
+        <f>UKData!B31</f>
+        <v>29</v>
+      </c>
+      <c r="C31" s="148">
+        <f>UKData!C31</f>
+        <v>1.9629315289040459</v>
+      </c>
+      <c r="D31" s="148">
+        <f>UKData!D31</f>
+        <v>1.0596772320910253</v>
+      </c>
+      <c r="E31" s="148">
+        <f>UKData!E31</f>
+        <v>2.5523349805870459</v>
+      </c>
+      <c r="F31" s="148">
+        <f>UKData!F31</f>
+        <v>0.99900000247902043</v>
+      </c>
+      <c r="G31" s="148">
+        <f>UKData!G31</f>
+        <v>0.98382437019791136</v>
+      </c>
+      <c r="H31" s="148" t="str">
+        <f>UKData!H31</f>
+        <v>NA</v>
+      </c>
+      <c r="I31" s="148"/>
+      <c r="J31" s="148"/>
+      <c r="K31" s="148"/>
+      <c r="L31" s="148"/>
+      <c r="M31" s="148">
+        <f>EXP(lambda_L*B31)</f>
+        <v>1.50080255245802</v>
+      </c>
+      <c r="N31" s="148">
+        <f>EXP(lambda_E*B31)</f>
+        <v>2.3869108535242765</v>
+      </c>
+      <c r="O31" s="148">
+        <f>E31^alpha * (M31*D31)^beta</f>
+        <v>1.8242103303833659</v>
+      </c>
+      <c r="P31" s="148">
+        <f>((1-gamma_E)^1 * O31^phi + gamma_E^1 * ($N31*F31)^phi)^invPhi</f>
+        <v>2.040240239089627</v>
+      </c>
+      <c r="Q31" s="148">
+        <f>((1-gamma_E)^1 * P31^phi + gamma_E^1 * ($N31*G31)^phi)^invPhi</f>
+        <v>2.1363285583131941</v>
+      </c>
+      <c r="R31" s="148"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="148">
+        <f>UKData!A32</f>
+        <v>2010</v>
+      </c>
+      <c r="B32" s="148">
+        <f>UKData!B32</f>
+        <v>30</v>
+      </c>
+      <c r="C32" s="148">
+        <f>UKData!C32</f>
+        <v>2.0039992695867763</v>
+      </c>
+      <c r="D32" s="148">
+        <f>UKData!D32</f>
+        <v>1.0649018924880995</v>
+      </c>
+      <c r="E32" s="148">
+        <f>UKData!E32</f>
+        <v>2.596944157292989</v>
+      </c>
+      <c r="F32" s="148">
+        <f>UKData!F32</f>
+        <v>1.0152842530613724</v>
+      </c>
+      <c r="G32" s="148">
+        <f>UKData!G32</f>
+        <v>1.0002896176350151</v>
+      </c>
+      <c r="H32" s="148" t="str">
+        <f>UKData!H32</f>
+        <v>NA</v>
+      </c>
+      <c r="I32" s="148"/>
+      <c r="J32" s="148"/>
+      <c r="K32" s="148"/>
+      <c r="L32" s="148"/>
+      <c r="M32" s="148">
+        <f>EXP(lambda_L*B32)</f>
+        <v>1.5219615556186337</v>
+      </c>
+      <c r="N32" s="148">
+        <f>EXP(lambda_E*B32)</f>
+        <v>2.4596031111569494</v>
+      </c>
+      <c r="O32" s="148">
+        <f>E32^alpha * (M32*D32)^beta</f>
+        <v>1.8581920037447974</v>
+      </c>
+      <c r="P32" s="148">
+        <f>((1-gamma_E)^1 * O32^phi + gamma_E^1 * ($N32*F32)^phi)^invPhi</f>
+        <v>2.1149173540547443</v>
+      </c>
+      <c r="Q32" s="148">
+        <f>((1-gamma_E)^1 * P32^phi + gamma_E^1 * ($N32*G32)^phi)^invPhi</f>
+        <v>2.2247150985167758</v>
+      </c>
+      <c r="R32" s="148"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="148">
+        <f>UKData!A33</f>
+        <v>2011</v>
+      </c>
+      <c r="B33" s="148">
+        <f>UKData!B33</f>
+        <v>31</v>
+      </c>
+      <c r="C33" s="148">
+        <f>UKData!C33</f>
+        <v>2.0171192742504478</v>
+      </c>
+      <c r="D33" s="148">
+        <f>UKData!D33</f>
+        <v>1.0633925461511669</v>
+      </c>
+      <c r="E33" s="148">
+        <f>UKData!E33</f>
+        <v>2.6357626243114307</v>
+      </c>
+      <c r="F33" s="148">
+        <f>UKData!F33</f>
+        <v>0.96688532466264787</v>
+      </c>
+      <c r="G33" s="148">
+        <f>UKData!G33</f>
+        <v>0.95181302656391054</v>
+      </c>
+      <c r="H33" s="148" t="str">
+        <f>UKData!H33</f>
+        <v>NA</v>
+      </c>
+      <c r="I33" s="148"/>
+      <c r="J33" s="148"/>
+      <c r="K33" s="148"/>
+      <c r="L33" s="148"/>
+      <c r="M33" s="148">
+        <f>EXP(lambda_L*B33)</f>
+        <v>1.5434188681164871</v>
+      </c>
+      <c r="N33" s="148">
+        <f>EXP(lambda_E*B33)</f>
+        <v>2.5345091776178545</v>
+      </c>
+      <c r="O33" s="148">
+        <f>E33^alpha * (M33*D33)^beta</f>
+        <v>1.8829500164335919</v>
+      </c>
+      <c r="P33" s="148">
+        <f>((1-gamma_E)^1 * O33^phi + gamma_E^1 * ($N33*F33)^phi)^invPhi</f>
+        <v>2.100346201569756</v>
+      </c>
+      <c r="Q33" s="148">
+        <f>((1-gamma_E)^1 * P33^phi + gamma_E^1 * ($N33*G33)^phi)^invPhi</f>
+        <v>2.1973055463908464</v>
+      </c>
+      <c r="R33" s="148"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="148"/>
+      <c r="B34" s="148"/>
+      <c r="C34" s="148"/>
+      <c r="D34" s="148"/>
+      <c r="E34" s="148"/>
+      <c r="F34" s="148"/>
+      <c r="G34" s="148"/>
+      <c r="H34" s="148"/>
+      <c r="I34" s="148"/>
+      <c r="J34" s="148"/>
+      <c r="K34" s="148"/>
+      <c r="L34" s="148"/>
+      <c r="M34" s="148"/>
+      <c r="N34" s="148"/>
+      <c r="O34" s="148"/>
+      <c r="P34" s="148"/>
+      <c r="Q34" s="148"/>
+      <c r="R34" s="148"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="148"/>
+      <c r="B35" s="148"/>
+      <c r="C35" s="148"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="148"/>
+      <c r="F35" s="148"/>
+      <c r="G35" s="148"/>
+      <c r="H35" s="148"/>
+      <c r="I35" s="148"/>
+      <c r="J35" s="148"/>
+      <c r="K35" s="148"/>
+      <c r="L35" s="148"/>
+      <c r="M35" s="148"/>
+      <c r="N35" s="148"/>
+      <c r="O35" s="148"/>
+      <c r="P35" s="148"/>
+      <c r="Q35" s="148"/>
+      <c r="R35" s="148"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="148"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="148"/>
+      <c r="H36" s="148"/>
+      <c r="I36" s="148"/>
+      <c r="J36" s="148"/>
+      <c r="K36" s="148"/>
+      <c r="L36" s="148"/>
+      <c r="M36" s="148"/>
+      <c r="N36" s="148"/>
+      <c r="O36" s="148"/>
+      <c r="P36" s="148"/>
+      <c r="Q36" s="148"/>
+      <c r="R36" s="148"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="148"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="148"/>
+      <c r="D37" s="148"/>
+      <c r="E37" s="148"/>
+      <c r="F37" s="148"/>
+      <c r="G37" s="148"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="148"/>
+      <c r="J37" s="148"/>
+      <c r="K37" s="148"/>
+      <c r="L37" s="148"/>
+      <c r="M37" s="148"/>
+      <c r="N37" s="148"/>
+      <c r="O37" s="148"/>
+      <c r="P37" s="148"/>
+      <c r="Q37" s="148"/>
+      <c r="R37" s="148"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="148"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="148"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="148"/>
+      <c r="F38" s="148"/>
+      <c r="G38" s="148"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="148"/>
+      <c r="J38" s="148"/>
+      <c r="K38" s="148"/>
+      <c r="L38" s="148"/>
+      <c r="M38" s="148"/>
+      <c r="N38" s="148"/>
+      <c r="O38" s="148"/>
+      <c r="P38" s="148"/>
+      <c r="Q38" s="148"/>
+      <c r="R38" s="148"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="148"/>
+      <c r="B39" s="148"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="148"/>
+      <c r="H39" s="148"/>
+      <c r="I39" s="148"/>
+      <c r="J39" s="148"/>
+      <c r="K39" s="148"/>
+      <c r="L39" s="148"/>
+      <c r="M39" s="148"/>
+      <c r="N39" s="148"/>
+      <c r="O39" s="148"/>
+      <c r="P39" s="148"/>
+      <c r="Q39" s="148"/>
+      <c r="R39" s="148"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="148"/>
+      <c r="B40" s="148"/>
+      <c r="C40" s="148"/>
+      <c r="D40" s="148"/>
+      <c r="E40" s="148"/>
+      <c r="F40" s="148"/>
+      <c r="G40" s="148"/>
+      <c r="H40" s="148"/>
+      <c r="I40" s="148"/>
+      <c r="J40" s="148"/>
+      <c r="K40" s="148"/>
+      <c r="L40" s="148"/>
+      <c r="M40" s="148"/>
+      <c r="N40" s="148"/>
+      <c r="O40" s="148"/>
+      <c r="P40" s="148"/>
+      <c r="Q40" s="148"/>
+      <c r="R40" s="148"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="148"/>
+      <c r="B41" s="148"/>
+      <c r="C41" s="148"/>
+      <c r="D41" s="148"/>
+      <c r="E41" s="148"/>
+      <c r="F41" s="148"/>
+      <c r="G41" s="148"/>
+      <c r="H41" s="148"/>
+      <c r="I41" s="148"/>
+      <c r="J41" s="148"/>
+      <c r="K41" s="148"/>
+      <c r="L41" s="148"/>
+      <c r="M41" s="148"/>
+      <c r="N41" s="148"/>
+      <c r="O41" s="148"/>
+      <c r="P41" s="148"/>
+      <c r="Q41" s="148"/>
+      <c r="R41" s="148"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="148"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="148"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="148"/>
+      <c r="G42" s="148"/>
+      <c r="H42" s="148"/>
+      <c r="I42" s="148"/>
+      <c r="J42" s="148"/>
+      <c r="K42" s="148"/>
+      <c r="L42" s="148"/>
+      <c r="M42" s="148"/>
+      <c r="N42" s="148"/>
+      <c r="O42" s="148"/>
+      <c r="P42" s="148"/>
+      <c r="Q42" s="148"/>
+      <c r="R42" s="148"/>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" s="148"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="148"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="148"/>
+      <c r="F43" s="148"/>
+      <c r="G43" s="148"/>
+      <c r="H43" s="148"/>
+      <c r="I43" s="148"/>
+      <c r="J43" s="148"/>
+      <c r="K43" s="148"/>
+      <c r="L43" s="148"/>
+      <c r="M43" s="148"/>
+      <c r="N43" s="148"/>
+      <c r="O43" s="148"/>
+      <c r="P43" s="148"/>
+      <c r="Q43" s="148"/>
+      <c r="R43" s="148"/>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" s="148"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="148"/>
+      <c r="D44" s="148"/>
+      <c r="E44" s="148"/>
+      <c r="F44" s="148"/>
+      <c r="G44" s="148"/>
+      <c r="H44" s="148"/>
+      <c r="I44" s="148"/>
+      <c r="J44" s="148"/>
+      <c r="K44" s="148"/>
+      <c r="L44" s="148"/>
+      <c r="M44" s="148"/>
+      <c r="N44" s="148"/>
+      <c r="O44" s="148"/>
+      <c r="P44" s="148"/>
+      <c r="Q44" s="148"/>
+      <c r="R44" s="148"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>